<commit_message>
alterando alguma coisa que não sei kkk
</commit_message>
<xml_diff>
--- a/dados/carga.xlsx
+++ b/dados/carga.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Aulas\Fundamentos de Linguagem Python para Análise de Dados e Data Science\23-Cap13\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\tecnoblimp.comparadados.e2e\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB01C789-9C84-4A85-BEEC-DD50188098A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFB8A09-76A2-4418-A2B3-124AFD96A4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{DA2F9FFA-A132-4463-9655-37FEAE11FC04}"/>
+    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{DA2F9FFA-A132-4463-9655-37FEAE11FC04}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -175,7 +175,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -281,7 +281,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -423,7 +423,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -434,7 +434,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,36 +497,36 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
-        <v>16635</v>
+        <v>16107</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4">
-        <v>61902</v>
+        <v>38045</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
-        <v>16107</v>
+        <v>16635</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5">
-        <v>38045</v>
+        <v>61902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>